<commit_message>
update OBM to provide supervisory control override option
</commit_message>
<xml_diff>
--- a/testbed/OBM/Master_Setup_AC_dense.xlsx
+++ b/testbed/OBM/Master_Setup_AC_dense.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repo\occ-behav-demand-flex\testbed\OBM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D484AF6-4698-40CB-82A3-AC73D9374B49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D71EAC9-7CBA-4FC4-95E8-A3FDD02AAB46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="12456" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="188">
   <si>
     <t>DEFINE GENERAL SIMULATION SETTINGS</t>
   </si>
@@ -1055,6 +1055,9 @@
       </rPr>
       <t xml:space="preserve"> = Agent-Based (full; Clo/Met adjust, real acceptability range)</t>
     </r>
+  </si>
+  <si>
+    <t>Thermostat reset interval (min)</t>
   </si>
 </sst>
 </file>
@@ -2402,80 +2405,80 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2836,7 +2839,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:Y74"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A67" workbookViewId="0">
       <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
@@ -2965,53 +2968,53 @@
       <c r="C14" s="146" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="191" t="s">
+      <c r="D14" s="173" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="192"/>
-      <c r="F14" s="192"/>
-      <c r="G14" s="192"/>
-      <c r="H14" s="192"/>
-      <c r="I14" s="192"/>
-      <c r="J14" s="192"/>
-      <c r="K14" s="192"/>
-      <c r="L14" s="192"/>
-      <c r="M14" s="193" t="s">
+      <c r="E14" s="174"/>
+      <c r="F14" s="174"/>
+      <c r="G14" s="174"/>
+      <c r="H14" s="174"/>
+      <c r="I14" s="174"/>
+      <c r="J14" s="174"/>
+      <c r="K14" s="174"/>
+      <c r="L14" s="174"/>
+      <c r="M14" s="175" t="s">
         <v>14</v>
       </c>
-      <c r="N14" s="194"/>
-      <c r="O14" s="194"/>
-      <c r="P14" s="194"/>
-      <c r="Q14" s="194"/>
-      <c r="R14" s="194"/>
-      <c r="S14" s="194"/>
-      <c r="T14" s="194"/>
-      <c r="U14" s="195"/>
-      <c r="V14" s="196"/>
-      <c r="W14" s="197"/>
-      <c r="X14" s="197"/>
-      <c r="Y14" s="197"/>
+      <c r="N14" s="176"/>
+      <c r="O14" s="176"/>
+      <c r="P14" s="176"/>
+      <c r="Q14" s="176"/>
+      <c r="R14" s="176"/>
+      <c r="S14" s="176"/>
+      <c r="T14" s="176"/>
+      <c r="U14" s="177"/>
+      <c r="V14" s="178"/>
+      <c r="W14" s="179"/>
+      <c r="X14" s="179"/>
+      <c r="Y14" s="179"/>
     </row>
     <row r="15" spans="1:25" ht="15" customHeight="1">
-      <c r="B15" s="182" t="s">
+      <c r="B15" s="189" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="187" t="s">
+      <c r="C15" s="194" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="179" t="s">
+      <c r="D15" s="180" t="s">
         <v>17</v>
       </c>
-      <c r="E15" s="180"/>
-      <c r="F15" s="180"/>
-      <c r="G15" s="180"/>
-      <c r="H15" s="180"/>
-      <c r="I15" s="181"/>
-      <c r="J15" s="179" t="s">
+      <c r="E15" s="181"/>
+      <c r="F15" s="181"/>
+      <c r="G15" s="181"/>
+      <c r="H15" s="181"/>
+      <c r="I15" s="182"/>
+      <c r="J15" s="180" t="s">
         <v>18</v>
       </c>
-      <c r="K15" s="180"/>
-      <c r="L15" s="181"/>
+      <c r="K15" s="181"/>
+      <c r="L15" s="182"/>
       <c r="M15" s="150" t="s">
         <v>19</v>
       </c>
@@ -3041,23 +3044,23 @@
       </c>
     </row>
     <row r="16" spans="1:25" ht="15" customHeight="1">
-      <c r="B16" s="183"/>
-      <c r="C16" s="174"/>
-      <c r="D16" s="176" t="s">
+      <c r="B16" s="190"/>
+      <c r="C16" s="195"/>
+      <c r="D16" s="183" t="s">
         <v>28</v>
       </c>
-      <c r="E16" s="177"/>
-      <c r="F16" s="178"/>
-      <c r="G16" s="176" t="s">
+      <c r="E16" s="184"/>
+      <c r="F16" s="185"/>
+      <c r="G16" s="183" t="s">
         <v>29</v>
       </c>
-      <c r="H16" s="177"/>
-      <c r="I16" s="178"/>
-      <c r="J16" s="176" t="s">
+      <c r="H16" s="184"/>
+      <c r="I16" s="185"/>
+      <c r="J16" s="183" t="s">
         <v>30</v>
       </c>
-      <c r="K16" s="177"/>
-      <c r="L16" s="178"/>
+      <c r="K16" s="184"/>
+      <c r="L16" s="185"/>
       <c r="M16" s="151">
         <v>2</v>
       </c>
@@ -3087,8 +3090,8 @@
       </c>
     </row>
     <row r="17" spans="2:21" ht="31.2">
-      <c r="B17" s="183"/>
-      <c r="C17" s="174"/>
+      <c r="B17" s="190"/>
+      <c r="C17" s="195"/>
       <c r="D17" s="147" t="s">
         <v>31</v>
       </c>
@@ -3133,8 +3136,8 @@
       <c r="U17" s="161"/>
     </row>
     <row r="18" spans="2:21">
-      <c r="B18" s="184"/>
-      <c r="C18" s="175"/>
+      <c r="B18" s="191"/>
+      <c r="C18" s="196"/>
       <c r="D18" s="148">
         <v>0</v>
       </c>
@@ -3179,25 +3182,25 @@
       <c r="U18" s="164"/>
     </row>
     <row r="19" spans="2:21" ht="18" customHeight="1">
-      <c r="B19" s="182" t="s">
+      <c r="B19" s="189" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="173" t="s">
+      <c r="C19" s="197" t="s">
         <v>38</v>
       </c>
-      <c r="D19" s="179" t="s">
+      <c r="D19" s="180" t="s">
         <v>17</v>
       </c>
-      <c r="E19" s="180"/>
-      <c r="F19" s="180"/>
-      <c r="G19" s="180"/>
-      <c r="H19" s="180"/>
-      <c r="I19" s="181"/>
-      <c r="J19" s="188" t="s">
+      <c r="E19" s="181"/>
+      <c r="F19" s="181"/>
+      <c r="G19" s="181"/>
+      <c r="H19" s="181"/>
+      <c r="I19" s="182"/>
+      <c r="J19" s="186" t="s">
         <v>18</v>
       </c>
-      <c r="K19" s="189"/>
-      <c r="L19" s="190"/>
+      <c r="K19" s="187"/>
+      <c r="L19" s="188"/>
       <c r="M19" s="147" t="s">
         <v>19</v>
       </c>
@@ -3227,23 +3230,23 @@
       </c>
     </row>
     <row r="20" spans="2:21" ht="15" customHeight="1">
-      <c r="B20" s="183"/>
-      <c r="C20" s="174"/>
-      <c r="D20" s="176" t="s">
+      <c r="B20" s="190"/>
+      <c r="C20" s="195"/>
+      <c r="D20" s="183" t="s">
         <v>28</v>
       </c>
-      <c r="E20" s="177"/>
-      <c r="F20" s="178"/>
-      <c r="G20" s="176" t="s">
+      <c r="E20" s="184"/>
+      <c r="F20" s="185"/>
+      <c r="G20" s="183" t="s">
         <v>29</v>
       </c>
-      <c r="H20" s="177"/>
-      <c r="I20" s="178"/>
-      <c r="J20" s="176" t="s">
+      <c r="H20" s="184"/>
+      <c r="I20" s="185"/>
+      <c r="J20" s="183" t="s">
         <v>30</v>
       </c>
-      <c r="K20" s="177"/>
-      <c r="L20" s="178"/>
+      <c r="K20" s="184"/>
+      <c r="L20" s="185"/>
       <c r="M20" s="151">
         <v>2</v>
       </c>
@@ -3273,8 +3276,8 @@
       </c>
     </row>
     <row r="21" spans="2:21" ht="31.2">
-      <c r="B21" s="183"/>
-      <c r="C21" s="174"/>
+      <c r="B21" s="190"/>
+      <c r="C21" s="195"/>
       <c r="D21" s="147" t="s">
         <v>31</v>
       </c>
@@ -3319,8 +3322,8 @@
       <c r="U21" s="161"/>
     </row>
     <row r="22" spans="2:21">
-      <c r="B22" s="184"/>
-      <c r="C22" s="175"/>
+      <c r="B22" s="191"/>
+      <c r="C22" s="196"/>
       <c r="D22" s="148">
         <v>0</v>
       </c>
@@ -3365,25 +3368,25 @@
       <c r="U22" s="164"/>
     </row>
     <row r="23" spans="2:21" ht="30" customHeight="1">
-      <c r="B23" s="185" t="s">
+      <c r="B23" s="192" t="s">
         <v>39</v>
       </c>
-      <c r="C23" s="173" t="s">
+      <c r="C23" s="197" t="s">
         <v>40</v>
       </c>
-      <c r="D23" s="179" t="s">
+      <c r="D23" s="180" t="s">
         <v>17</v>
       </c>
-      <c r="E23" s="180"/>
-      <c r="F23" s="180"/>
-      <c r="G23" s="180"/>
-      <c r="H23" s="180"/>
-      <c r="I23" s="181"/>
-      <c r="J23" s="179" t="s">
+      <c r="E23" s="181"/>
+      <c r="F23" s="181"/>
+      <c r="G23" s="181"/>
+      <c r="H23" s="181"/>
+      <c r="I23" s="182"/>
+      <c r="J23" s="180" t="s">
         <v>18</v>
       </c>
-      <c r="K23" s="180"/>
-      <c r="L23" s="181"/>
+      <c r="K23" s="181"/>
+      <c r="L23" s="182"/>
       <c r="M23" s="147" t="s">
         <v>19</v>
       </c>
@@ -3413,23 +3416,23 @@
       </c>
     </row>
     <row r="24" spans="2:21" ht="15" customHeight="1">
-      <c r="B24" s="183"/>
-      <c r="C24" s="174"/>
-      <c r="D24" s="176" t="s">
+      <c r="B24" s="190"/>
+      <c r="C24" s="195"/>
+      <c r="D24" s="183" t="s">
         <v>28</v>
       </c>
-      <c r="E24" s="177"/>
-      <c r="F24" s="178"/>
-      <c r="G24" s="176" t="s">
+      <c r="E24" s="184"/>
+      <c r="F24" s="185"/>
+      <c r="G24" s="183" t="s">
         <v>29</v>
       </c>
-      <c r="H24" s="177"/>
-      <c r="I24" s="178"/>
-      <c r="J24" s="176" t="s">
+      <c r="H24" s="184"/>
+      <c r="I24" s="185"/>
+      <c r="J24" s="183" t="s">
         <v>30</v>
       </c>
-      <c r="K24" s="177"/>
-      <c r="L24" s="178"/>
+      <c r="K24" s="184"/>
+      <c r="L24" s="185"/>
       <c r="M24" s="151">
         <v>2</v>
       </c>
@@ -3459,8 +3462,8 @@
       </c>
     </row>
     <row r="25" spans="2:21" ht="31.2">
-      <c r="B25" s="183"/>
-      <c r="C25" s="174"/>
+      <c r="B25" s="190"/>
+      <c r="C25" s="195"/>
       <c r="D25" s="147" t="s">
         <v>31</v>
       </c>
@@ -3505,8 +3508,8 @@
       <c r="U25" s="161"/>
     </row>
     <row r="26" spans="2:21">
-      <c r="B26" s="184"/>
-      <c r="C26" s="175"/>
+      <c r="B26" s="191"/>
+      <c r="C26" s="196"/>
       <c r="D26" s="148">
         <v>0</v>
       </c>
@@ -3551,25 +3554,25 @@
       <c r="U26" s="164"/>
     </row>
     <row r="27" spans="2:21" ht="30" customHeight="1">
-      <c r="B27" s="185" t="s">
+      <c r="B27" s="192" t="s">
         <v>41</v>
       </c>
-      <c r="C27" s="173" t="s">
+      <c r="C27" s="197" t="s">
         <v>42</v>
       </c>
-      <c r="D27" s="179" t="s">
+      <c r="D27" s="180" t="s">
         <v>17</v>
       </c>
-      <c r="E27" s="180"/>
-      <c r="F27" s="180"/>
-      <c r="G27" s="180"/>
-      <c r="H27" s="180"/>
-      <c r="I27" s="181"/>
-      <c r="J27" s="179" t="s">
+      <c r="E27" s="181"/>
+      <c r="F27" s="181"/>
+      <c r="G27" s="181"/>
+      <c r="H27" s="181"/>
+      <c r="I27" s="182"/>
+      <c r="J27" s="180" t="s">
         <v>18</v>
       </c>
-      <c r="K27" s="180"/>
-      <c r="L27" s="181"/>
+      <c r="K27" s="181"/>
+      <c r="L27" s="182"/>
       <c r="M27" s="147" t="s">
         <v>19</v>
       </c>
@@ -3599,23 +3602,23 @@
       </c>
     </row>
     <row r="28" spans="2:21" ht="15" customHeight="1">
-      <c r="B28" s="183"/>
-      <c r="C28" s="174"/>
-      <c r="D28" s="176" t="s">
+      <c r="B28" s="190"/>
+      <c r="C28" s="195"/>
+      <c r="D28" s="183" t="s">
         <v>28</v>
       </c>
-      <c r="E28" s="177"/>
-      <c r="F28" s="178"/>
-      <c r="G28" s="176" t="s">
+      <c r="E28" s="184"/>
+      <c r="F28" s="185"/>
+      <c r="G28" s="183" t="s">
         <v>29</v>
       </c>
-      <c r="H28" s="177"/>
-      <c r="I28" s="178"/>
-      <c r="J28" s="176" t="s">
+      <c r="H28" s="184"/>
+      <c r="I28" s="185"/>
+      <c r="J28" s="183" t="s">
         <v>30</v>
       </c>
-      <c r="K28" s="177"/>
-      <c r="L28" s="178"/>
+      <c r="K28" s="184"/>
+      <c r="L28" s="185"/>
       <c r="M28" s="151">
         <v>2</v>
       </c>
@@ -3645,8 +3648,8 @@
       </c>
     </row>
     <row r="29" spans="2:21" ht="31.2">
-      <c r="B29" s="183"/>
-      <c r="C29" s="174"/>
+      <c r="B29" s="190"/>
+      <c r="C29" s="195"/>
       <c r="D29" s="147" t="s">
         <v>31</v>
       </c>
@@ -3691,8 +3694,8 @@
       <c r="U29" s="161"/>
     </row>
     <row r="30" spans="2:21">
-      <c r="B30" s="184"/>
-      <c r="C30" s="175"/>
+      <c r="B30" s="191"/>
+      <c r="C30" s="196"/>
       <c r="D30" s="148">
         <v>0</v>
       </c>
@@ -3737,25 +3740,25 @@
       <c r="U30" s="164"/>
     </row>
     <row r="31" spans="2:21">
-      <c r="B31" s="185" t="s">
+      <c r="B31" s="192" t="s">
         <v>43</v>
       </c>
-      <c r="C31" s="173">
+      <c r="C31" s="197">
         <v>5</v>
       </c>
-      <c r="D31" s="179" t="s">
+      <c r="D31" s="180" t="s">
         <v>17</v>
       </c>
-      <c r="E31" s="180"/>
-      <c r="F31" s="180"/>
-      <c r="G31" s="180"/>
-      <c r="H31" s="180"/>
-      <c r="I31" s="181"/>
-      <c r="J31" s="179" t="s">
+      <c r="E31" s="181"/>
+      <c r="F31" s="181"/>
+      <c r="G31" s="181"/>
+      <c r="H31" s="181"/>
+      <c r="I31" s="182"/>
+      <c r="J31" s="180" t="s">
         <v>18</v>
       </c>
-      <c r="K31" s="180"/>
-      <c r="L31" s="181"/>
+      <c r="K31" s="181"/>
+      <c r="L31" s="182"/>
       <c r="M31" s="147" t="s">
         <v>19</v>
       </c>
@@ -3785,23 +3788,23 @@
       </c>
     </row>
     <row r="32" spans="2:21" ht="15" customHeight="1">
-      <c r="B32" s="183"/>
-      <c r="C32" s="174"/>
-      <c r="D32" s="176" t="s">
+      <c r="B32" s="190"/>
+      <c r="C32" s="195"/>
+      <c r="D32" s="183" t="s">
         <v>28</v>
       </c>
-      <c r="E32" s="177"/>
-      <c r="F32" s="178"/>
-      <c r="G32" s="176" t="s">
+      <c r="E32" s="184"/>
+      <c r="F32" s="185"/>
+      <c r="G32" s="183" t="s">
         <v>29</v>
       </c>
-      <c r="H32" s="177"/>
-      <c r="I32" s="178"/>
-      <c r="J32" s="176" t="s">
+      <c r="H32" s="184"/>
+      <c r="I32" s="185"/>
+      <c r="J32" s="183" t="s">
         <v>30</v>
       </c>
-      <c r="K32" s="177"/>
-      <c r="L32" s="178"/>
+      <c r="K32" s="184"/>
+      <c r="L32" s="185"/>
       <c r="M32" s="151">
         <v>2</v>
       </c>
@@ -3831,8 +3834,8 @@
       </c>
     </row>
     <row r="33" spans="2:21" ht="31.2">
-      <c r="B33" s="183"/>
-      <c r="C33" s="174"/>
+      <c r="B33" s="190"/>
+      <c r="C33" s="195"/>
       <c r="D33" s="147" t="s">
         <v>31</v>
       </c>
@@ -3877,8 +3880,8 @@
       <c r="U33" s="161"/>
     </row>
     <row r="34" spans="2:21">
-      <c r="B34" s="184"/>
-      <c r="C34" s="175"/>
+      <c r="B34" s="191"/>
+      <c r="C34" s="196"/>
       <c r="D34" s="148">
         <v>0</v>
       </c>
@@ -3923,25 +3926,25 @@
       <c r="U34" s="164"/>
     </row>
     <row r="35" spans="2:21">
-      <c r="B35" s="185" t="s">
+      <c r="B35" s="192" t="s">
         <v>44</v>
       </c>
-      <c r="C35" s="173">
+      <c r="C35" s="197">
         <v>6</v>
       </c>
-      <c r="D35" s="179" t="s">
+      <c r="D35" s="180" t="s">
         <v>17</v>
       </c>
-      <c r="E35" s="180"/>
-      <c r="F35" s="180"/>
-      <c r="G35" s="180"/>
-      <c r="H35" s="180"/>
-      <c r="I35" s="181"/>
-      <c r="J35" s="179" t="s">
+      <c r="E35" s="181"/>
+      <c r="F35" s="181"/>
+      <c r="G35" s="181"/>
+      <c r="H35" s="181"/>
+      <c r="I35" s="182"/>
+      <c r="J35" s="180" t="s">
         <v>18</v>
       </c>
-      <c r="K35" s="180"/>
-      <c r="L35" s="181"/>
+      <c r="K35" s="181"/>
+      <c r="L35" s="182"/>
       <c r="M35" s="155" t="s">
         <v>19</v>
       </c>
@@ -3971,23 +3974,23 @@
       </c>
     </row>
     <row r="36" spans="2:21" ht="15" customHeight="1">
-      <c r="B36" s="183"/>
-      <c r="C36" s="174"/>
-      <c r="D36" s="176" t="s">
+      <c r="B36" s="190"/>
+      <c r="C36" s="195"/>
+      <c r="D36" s="183" t="s">
         <v>28</v>
       </c>
-      <c r="E36" s="177"/>
-      <c r="F36" s="178"/>
-      <c r="G36" s="176" t="s">
+      <c r="E36" s="184"/>
+      <c r="F36" s="185"/>
+      <c r="G36" s="183" t="s">
         <v>29</v>
       </c>
-      <c r="H36" s="177"/>
-      <c r="I36" s="178"/>
-      <c r="J36" s="176" t="s">
+      <c r="H36" s="184"/>
+      <c r="I36" s="185"/>
+      <c r="J36" s="183" t="s">
         <v>30</v>
       </c>
-      <c r="K36" s="177"/>
-      <c r="L36" s="178"/>
+      <c r="K36" s="184"/>
+      <c r="L36" s="185"/>
       <c r="M36" s="151">
         <v>2</v>
       </c>
@@ -4017,8 +4020,8 @@
       </c>
     </row>
     <row r="37" spans="2:21" ht="31.2">
-      <c r="B37" s="183"/>
-      <c r="C37" s="174"/>
+      <c r="B37" s="190"/>
+      <c r="C37" s="195"/>
       <c r="D37" s="147" t="s">
         <v>31</v>
       </c>
@@ -4063,8 +4066,8 @@
       <c r="U37" s="161"/>
     </row>
     <row r="38" spans="2:21">
-      <c r="B38" s="186"/>
-      <c r="C38" s="175"/>
+      <c r="B38" s="193"/>
+      <c r="C38" s="196"/>
       <c r="D38" s="148">
         <v>0</v>
       </c>
@@ -4109,25 +4112,25 @@
       <c r="U38" s="164"/>
     </row>
     <row r="39" spans="2:21">
-      <c r="B39" s="182" t="s">
+      <c r="B39" s="189" t="s">
         <v>45</v>
       </c>
-      <c r="C39" s="173">
+      <c r="C39" s="197">
         <v>7</v>
       </c>
-      <c r="D39" s="179" t="s">
+      <c r="D39" s="180" t="s">
         <v>17</v>
       </c>
-      <c r="E39" s="180"/>
-      <c r="F39" s="180"/>
-      <c r="G39" s="180"/>
-      <c r="H39" s="180"/>
-      <c r="I39" s="181"/>
-      <c r="J39" s="188" t="s">
+      <c r="E39" s="181"/>
+      <c r="F39" s="181"/>
+      <c r="G39" s="181"/>
+      <c r="H39" s="181"/>
+      <c r="I39" s="182"/>
+      <c r="J39" s="186" t="s">
         <v>18</v>
       </c>
-      <c r="K39" s="189"/>
-      <c r="L39" s="190"/>
+      <c r="K39" s="187"/>
+      <c r="L39" s="188"/>
       <c r="M39" s="147" t="s">
         <v>19</v>
       </c>
@@ -4157,23 +4160,23 @@
       </c>
     </row>
     <row r="40" spans="2:21" ht="15" customHeight="1">
-      <c r="B40" s="183"/>
-      <c r="C40" s="174"/>
-      <c r="D40" s="176" t="s">
+      <c r="B40" s="190"/>
+      <c r="C40" s="195"/>
+      <c r="D40" s="183" t="s">
         <v>28</v>
       </c>
-      <c r="E40" s="177"/>
-      <c r="F40" s="178"/>
-      <c r="G40" s="176" t="s">
+      <c r="E40" s="184"/>
+      <c r="F40" s="185"/>
+      <c r="G40" s="183" t="s">
         <v>29</v>
       </c>
-      <c r="H40" s="177"/>
-      <c r="I40" s="178"/>
-      <c r="J40" s="176" t="s">
+      <c r="H40" s="184"/>
+      <c r="I40" s="185"/>
+      <c r="J40" s="183" t="s">
         <v>30</v>
       </c>
-      <c r="K40" s="177"/>
-      <c r="L40" s="178"/>
+      <c r="K40" s="184"/>
+      <c r="L40" s="185"/>
       <c r="M40" s="151">
         <v>2</v>
       </c>
@@ -4203,8 +4206,8 @@
       </c>
     </row>
     <row r="41" spans="2:21" ht="31.2">
-      <c r="B41" s="183"/>
-      <c r="C41" s="174"/>
+      <c r="B41" s="190"/>
+      <c r="C41" s="195"/>
       <c r="D41" s="147" t="s">
         <v>31</v>
       </c>
@@ -4249,8 +4252,8 @@
       <c r="U41" s="161"/>
     </row>
     <row r="42" spans="2:21">
-      <c r="B42" s="184"/>
-      <c r="C42" s="175"/>
+      <c r="B42" s="191"/>
+      <c r="C42" s="196"/>
       <c r="D42" s="148">
         <v>0</v>
       </c>
@@ -4295,25 +4298,25 @@
       <c r="U42" s="164"/>
     </row>
     <row r="43" spans="2:21">
-      <c r="B43" s="185" t="s">
+      <c r="B43" s="192" t="s">
         <v>46</v>
       </c>
-      <c r="C43" s="173">
+      <c r="C43" s="197">
         <v>8</v>
       </c>
-      <c r="D43" s="179" t="s">
+      <c r="D43" s="180" t="s">
         <v>17</v>
       </c>
-      <c r="E43" s="180"/>
-      <c r="F43" s="180"/>
-      <c r="G43" s="180"/>
-      <c r="H43" s="180"/>
-      <c r="I43" s="181"/>
-      <c r="J43" s="179" t="s">
+      <c r="E43" s="181"/>
+      <c r="F43" s="181"/>
+      <c r="G43" s="181"/>
+      <c r="H43" s="181"/>
+      <c r="I43" s="182"/>
+      <c r="J43" s="180" t="s">
         <v>18</v>
       </c>
-      <c r="K43" s="180"/>
-      <c r="L43" s="181"/>
+      <c r="K43" s="181"/>
+      <c r="L43" s="182"/>
       <c r="M43" s="147" t="s">
         <v>19</v>
       </c>
@@ -4343,23 +4346,23 @@
       </c>
     </row>
     <row r="44" spans="2:21" ht="15" customHeight="1">
-      <c r="B44" s="183"/>
-      <c r="C44" s="174"/>
-      <c r="D44" s="176" t="s">
+      <c r="B44" s="190"/>
+      <c r="C44" s="195"/>
+      <c r="D44" s="183" t="s">
         <v>28</v>
       </c>
-      <c r="E44" s="177"/>
-      <c r="F44" s="178"/>
-      <c r="G44" s="176" t="s">
+      <c r="E44" s="184"/>
+      <c r="F44" s="185"/>
+      <c r="G44" s="183" t="s">
         <v>29</v>
       </c>
-      <c r="H44" s="177"/>
-      <c r="I44" s="178"/>
-      <c r="J44" s="176" t="s">
+      <c r="H44" s="184"/>
+      <c r="I44" s="185"/>
+      <c r="J44" s="183" t="s">
         <v>30</v>
       </c>
-      <c r="K44" s="177"/>
-      <c r="L44" s="178"/>
+      <c r="K44" s="184"/>
+      <c r="L44" s="185"/>
       <c r="M44" s="151">
         <v>2</v>
       </c>
@@ -4389,8 +4392,8 @@
       </c>
     </row>
     <row r="45" spans="2:21" ht="31.2">
-      <c r="B45" s="183"/>
-      <c r="C45" s="174"/>
+      <c r="B45" s="190"/>
+      <c r="C45" s="195"/>
       <c r="D45" s="147" t="s">
         <v>31</v>
       </c>
@@ -4435,8 +4438,8 @@
       <c r="U45" s="161"/>
     </row>
     <row r="46" spans="2:21">
-      <c r="B46" s="184"/>
-      <c r="C46" s="175"/>
+      <c r="B46" s="191"/>
+      <c r="C46" s="196"/>
       <c r="D46" s="148">
         <v>0</v>
       </c>
@@ -4481,25 +4484,25 @@
       <c r="U46" s="164"/>
     </row>
     <row r="47" spans="2:21">
-      <c r="B47" s="185" t="s">
+      <c r="B47" s="192" t="s">
         <v>47</v>
       </c>
-      <c r="C47" s="173">
+      <c r="C47" s="197">
         <v>9</v>
       </c>
-      <c r="D47" s="179" t="s">
+      <c r="D47" s="180" t="s">
         <v>17</v>
       </c>
-      <c r="E47" s="180"/>
-      <c r="F47" s="180"/>
-      <c r="G47" s="180"/>
-      <c r="H47" s="180"/>
-      <c r="I47" s="181"/>
-      <c r="J47" s="179" t="s">
+      <c r="E47" s="181"/>
+      <c r="F47" s="181"/>
+      <c r="G47" s="181"/>
+      <c r="H47" s="181"/>
+      <c r="I47" s="182"/>
+      <c r="J47" s="180" t="s">
         <v>18</v>
       </c>
-      <c r="K47" s="180"/>
-      <c r="L47" s="181"/>
+      <c r="K47" s="181"/>
+      <c r="L47" s="182"/>
       <c r="M47" s="147" t="s">
         <v>19</v>
       </c>
@@ -4529,23 +4532,23 @@
       </c>
     </row>
     <row r="48" spans="2:21" ht="15" customHeight="1">
-      <c r="B48" s="183"/>
-      <c r="C48" s="174"/>
-      <c r="D48" s="176" t="s">
+      <c r="B48" s="190"/>
+      <c r="C48" s="195"/>
+      <c r="D48" s="183" t="s">
         <v>28</v>
       </c>
-      <c r="E48" s="177"/>
-      <c r="F48" s="178"/>
-      <c r="G48" s="176" t="s">
+      <c r="E48" s="184"/>
+      <c r="F48" s="185"/>
+      <c r="G48" s="183" t="s">
         <v>29</v>
       </c>
-      <c r="H48" s="177"/>
-      <c r="I48" s="178"/>
-      <c r="J48" s="176" t="s">
+      <c r="H48" s="184"/>
+      <c r="I48" s="185"/>
+      <c r="J48" s="183" t="s">
         <v>30</v>
       </c>
-      <c r="K48" s="177"/>
-      <c r="L48" s="178"/>
+      <c r="K48" s="184"/>
+      <c r="L48" s="185"/>
       <c r="M48" s="151">
         <v>2</v>
       </c>
@@ -4575,8 +4578,8 @@
       </c>
     </row>
     <row r="49" spans="2:21" ht="31.2">
-      <c r="B49" s="183"/>
-      <c r="C49" s="174"/>
+      <c r="B49" s="190"/>
+      <c r="C49" s="195"/>
       <c r="D49" s="147" t="s">
         <v>31</v>
       </c>
@@ -4621,8 +4624,8 @@
       <c r="U49" s="161"/>
     </row>
     <row r="50" spans="2:21">
-      <c r="B50" s="184"/>
-      <c r="C50" s="175"/>
+      <c r="B50" s="191"/>
+      <c r="C50" s="196"/>
       <c r="D50" s="148">
         <v>0</v>
       </c>
@@ -4667,25 +4670,25 @@
       <c r="U50" s="164"/>
     </row>
     <row r="51" spans="2:21">
-      <c r="B51" s="185" t="s">
+      <c r="B51" s="192" t="s">
         <v>48</v>
       </c>
-      <c r="C51" s="173">
+      <c r="C51" s="197">
         <v>10</v>
       </c>
-      <c r="D51" s="179" t="s">
+      <c r="D51" s="180" t="s">
         <v>17</v>
       </c>
-      <c r="E51" s="180"/>
-      <c r="F51" s="180"/>
-      <c r="G51" s="180"/>
-      <c r="H51" s="180"/>
-      <c r="I51" s="181"/>
-      <c r="J51" s="179" t="s">
+      <c r="E51" s="181"/>
+      <c r="F51" s="181"/>
+      <c r="G51" s="181"/>
+      <c r="H51" s="181"/>
+      <c r="I51" s="182"/>
+      <c r="J51" s="180" t="s">
         <v>18</v>
       </c>
-      <c r="K51" s="180"/>
-      <c r="L51" s="181"/>
+      <c r="K51" s="181"/>
+      <c r="L51" s="182"/>
       <c r="M51" s="147" t="s">
         <v>19</v>
       </c>
@@ -4715,23 +4718,23 @@
       </c>
     </row>
     <row r="52" spans="2:21" ht="15" customHeight="1">
-      <c r="B52" s="183"/>
-      <c r="C52" s="174"/>
-      <c r="D52" s="176" t="s">
+      <c r="B52" s="190"/>
+      <c r="C52" s="195"/>
+      <c r="D52" s="183" t="s">
         <v>28</v>
       </c>
-      <c r="E52" s="177"/>
-      <c r="F52" s="178"/>
-      <c r="G52" s="176" t="s">
+      <c r="E52" s="184"/>
+      <c r="F52" s="185"/>
+      <c r="G52" s="183" t="s">
         <v>29</v>
       </c>
-      <c r="H52" s="177"/>
-      <c r="I52" s="178"/>
-      <c r="J52" s="176" t="s">
+      <c r="H52" s="184"/>
+      <c r="I52" s="185"/>
+      <c r="J52" s="183" t="s">
         <v>30</v>
       </c>
-      <c r="K52" s="177"/>
-      <c r="L52" s="178"/>
+      <c r="K52" s="184"/>
+      <c r="L52" s="185"/>
       <c r="M52" s="151">
         <v>2</v>
       </c>
@@ -4761,8 +4764,8 @@
       </c>
     </row>
     <row r="53" spans="2:21" ht="31.2">
-      <c r="B53" s="183"/>
-      <c r="C53" s="174"/>
+      <c r="B53" s="190"/>
+      <c r="C53" s="195"/>
       <c r="D53" s="147" t="s">
         <v>31</v>
       </c>
@@ -4807,8 +4810,8 @@
       <c r="U53" s="161"/>
     </row>
     <row r="54" spans="2:21">
-      <c r="B54" s="184"/>
-      <c r="C54" s="175"/>
+      <c r="B54" s="191"/>
+      <c r="C54" s="196"/>
       <c r="D54" s="148">
         <v>0</v>
       </c>
@@ -4853,25 +4856,25 @@
       <c r="U54" s="164"/>
     </row>
     <row r="55" spans="2:21">
-      <c r="B55" s="185" t="s">
+      <c r="B55" s="192" t="s">
         <v>49</v>
       </c>
-      <c r="C55" s="173">
+      <c r="C55" s="197">
         <v>11</v>
       </c>
-      <c r="D55" s="179" t="s">
+      <c r="D55" s="180" t="s">
         <v>17</v>
       </c>
-      <c r="E55" s="180"/>
-      <c r="F55" s="180"/>
-      <c r="G55" s="180"/>
-      <c r="H55" s="180"/>
-      <c r="I55" s="181"/>
-      <c r="J55" s="179" t="s">
+      <c r="E55" s="181"/>
+      <c r="F55" s="181"/>
+      <c r="G55" s="181"/>
+      <c r="H55" s="181"/>
+      <c r="I55" s="182"/>
+      <c r="J55" s="180" t="s">
         <v>18</v>
       </c>
-      <c r="K55" s="180"/>
-      <c r="L55" s="181"/>
+      <c r="K55" s="181"/>
+      <c r="L55" s="182"/>
       <c r="M55" s="155" t="s">
         <v>19</v>
       </c>
@@ -4901,23 +4904,23 @@
       </c>
     </row>
     <row r="56" spans="2:21" ht="15" customHeight="1">
-      <c r="B56" s="183"/>
-      <c r="C56" s="174"/>
-      <c r="D56" s="176" t="s">
+      <c r="B56" s="190"/>
+      <c r="C56" s="195"/>
+      <c r="D56" s="183" t="s">
         <v>28</v>
       </c>
-      <c r="E56" s="177"/>
-      <c r="F56" s="178"/>
-      <c r="G56" s="176" t="s">
+      <c r="E56" s="184"/>
+      <c r="F56" s="185"/>
+      <c r="G56" s="183" t="s">
         <v>29</v>
       </c>
-      <c r="H56" s="177"/>
-      <c r="I56" s="178"/>
-      <c r="J56" s="176" t="s">
+      <c r="H56" s="184"/>
+      <c r="I56" s="185"/>
+      <c r="J56" s="183" t="s">
         <v>30</v>
       </c>
-      <c r="K56" s="177"/>
-      <c r="L56" s="178"/>
+      <c r="K56" s="184"/>
+      <c r="L56" s="185"/>
       <c r="M56" s="151">
         <v>2</v>
       </c>
@@ -4947,8 +4950,8 @@
       </c>
     </row>
     <row r="57" spans="2:21" ht="31.2">
-      <c r="B57" s="183"/>
-      <c r="C57" s="174"/>
+      <c r="B57" s="190"/>
+      <c r="C57" s="195"/>
       <c r="D57" s="147" t="s">
         <v>31</v>
       </c>
@@ -4993,8 +4996,8 @@
       <c r="U57" s="161"/>
     </row>
     <row r="58" spans="2:21">
-      <c r="B58" s="186"/>
-      <c r="C58" s="175"/>
+      <c r="B58" s="193"/>
+      <c r="C58" s="196"/>
       <c r="D58" s="148">
         <v>0</v>
       </c>
@@ -5039,25 +5042,25 @@
       <c r="U58" s="164"/>
     </row>
     <row r="59" spans="2:21">
-      <c r="B59" s="182" t="s">
+      <c r="B59" s="189" t="s">
         <v>50</v>
       </c>
-      <c r="C59" s="173">
+      <c r="C59" s="197">
         <v>12</v>
       </c>
-      <c r="D59" s="179" t="s">
+      <c r="D59" s="180" t="s">
         <v>17</v>
       </c>
-      <c r="E59" s="180"/>
-      <c r="F59" s="180"/>
-      <c r="G59" s="180"/>
-      <c r="H59" s="180"/>
-      <c r="I59" s="181"/>
-      <c r="J59" s="188" t="s">
+      <c r="E59" s="181"/>
+      <c r="F59" s="181"/>
+      <c r="G59" s="181"/>
+      <c r="H59" s="181"/>
+      <c r="I59" s="182"/>
+      <c r="J59" s="186" t="s">
         <v>18</v>
       </c>
-      <c r="K59" s="189"/>
-      <c r="L59" s="190"/>
+      <c r="K59" s="187"/>
+      <c r="L59" s="188"/>
       <c r="M59" s="147" t="s">
         <v>19</v>
       </c>
@@ -5087,23 +5090,23 @@
       </c>
     </row>
     <row r="60" spans="2:21" ht="15" customHeight="1">
-      <c r="B60" s="183"/>
-      <c r="C60" s="174"/>
-      <c r="D60" s="176" t="s">
+      <c r="B60" s="190"/>
+      <c r="C60" s="195"/>
+      <c r="D60" s="183" t="s">
         <v>28</v>
       </c>
-      <c r="E60" s="177"/>
-      <c r="F60" s="178"/>
-      <c r="G60" s="176" t="s">
+      <c r="E60" s="184"/>
+      <c r="F60" s="185"/>
+      <c r="G60" s="183" t="s">
         <v>29</v>
       </c>
-      <c r="H60" s="177"/>
-      <c r="I60" s="178"/>
-      <c r="J60" s="176" t="s">
+      <c r="H60" s="184"/>
+      <c r="I60" s="185"/>
+      <c r="J60" s="183" t="s">
         <v>30</v>
       </c>
-      <c r="K60" s="177"/>
-      <c r="L60" s="178"/>
+      <c r="K60" s="184"/>
+      <c r="L60" s="185"/>
       <c r="M60" s="151">
         <v>2</v>
       </c>
@@ -5133,8 +5136,8 @@
       </c>
     </row>
     <row r="61" spans="2:21" ht="31.2">
-      <c r="B61" s="183"/>
-      <c r="C61" s="174"/>
+      <c r="B61" s="190"/>
+      <c r="C61" s="195"/>
       <c r="D61" s="147" t="s">
         <v>31</v>
       </c>
@@ -5179,8 +5182,8 @@
       <c r="U61" s="161"/>
     </row>
     <row r="62" spans="2:21">
-      <c r="B62" s="184"/>
-      <c r="C62" s="175"/>
+      <c r="B62" s="191"/>
+      <c r="C62" s="196"/>
       <c r="D62" s="148">
         <v>0</v>
       </c>
@@ -5225,25 +5228,25 @@
       <c r="U62" s="164"/>
     </row>
     <row r="63" spans="2:21">
-      <c r="B63" s="185" t="s">
+      <c r="B63" s="192" t="s">
         <v>51</v>
       </c>
-      <c r="C63" s="173">
+      <c r="C63" s="197">
         <v>13</v>
       </c>
-      <c r="D63" s="179" t="s">
+      <c r="D63" s="180" t="s">
         <v>17</v>
       </c>
-      <c r="E63" s="180"/>
-      <c r="F63" s="180"/>
-      <c r="G63" s="180"/>
-      <c r="H63" s="180"/>
-      <c r="I63" s="181"/>
-      <c r="J63" s="179" t="s">
+      <c r="E63" s="181"/>
+      <c r="F63" s="181"/>
+      <c r="G63" s="181"/>
+      <c r="H63" s="181"/>
+      <c r="I63" s="182"/>
+      <c r="J63" s="180" t="s">
         <v>18</v>
       </c>
-      <c r="K63" s="180"/>
-      <c r="L63" s="181"/>
+      <c r="K63" s="181"/>
+      <c r="L63" s="182"/>
       <c r="M63" s="147" t="s">
         <v>19</v>
       </c>
@@ -5273,23 +5276,23 @@
       </c>
     </row>
     <row r="64" spans="2:21" ht="15" customHeight="1">
-      <c r="B64" s="183"/>
-      <c r="C64" s="174"/>
-      <c r="D64" s="176" t="s">
+      <c r="B64" s="190"/>
+      <c r="C64" s="195"/>
+      <c r="D64" s="183" t="s">
         <v>28</v>
       </c>
-      <c r="E64" s="177"/>
-      <c r="F64" s="178"/>
-      <c r="G64" s="176" t="s">
+      <c r="E64" s="184"/>
+      <c r="F64" s="185"/>
+      <c r="G64" s="183" t="s">
         <v>29</v>
       </c>
-      <c r="H64" s="177"/>
-      <c r="I64" s="178"/>
-      <c r="J64" s="176" t="s">
+      <c r="H64" s="184"/>
+      <c r="I64" s="185"/>
+      <c r="J64" s="183" t="s">
         <v>30</v>
       </c>
-      <c r="K64" s="177"/>
-      <c r="L64" s="178"/>
+      <c r="K64" s="184"/>
+      <c r="L64" s="185"/>
       <c r="M64" s="151">
         <v>2</v>
       </c>
@@ -5319,8 +5322,8 @@
       </c>
     </row>
     <row r="65" spans="2:21" ht="31.2">
-      <c r="B65" s="183"/>
-      <c r="C65" s="174"/>
+      <c r="B65" s="190"/>
+      <c r="C65" s="195"/>
       <c r="D65" s="147" t="s">
         <v>31</v>
       </c>
@@ -5365,8 +5368,8 @@
       <c r="U65" s="161"/>
     </row>
     <row r="66" spans="2:21">
-      <c r="B66" s="184"/>
-      <c r="C66" s="175"/>
+      <c r="B66" s="191"/>
+      <c r="C66" s="196"/>
       <c r="D66" s="148">
         <v>0</v>
       </c>
@@ -5411,25 +5414,25 @@
       <c r="U66" s="164"/>
     </row>
     <row r="67" spans="2:21">
-      <c r="B67" s="185" t="s">
+      <c r="B67" s="192" t="s">
         <v>52</v>
       </c>
-      <c r="C67" s="173">
+      <c r="C67" s="197">
         <v>14</v>
       </c>
-      <c r="D67" s="179" t="s">
+      <c r="D67" s="180" t="s">
         <v>17</v>
       </c>
-      <c r="E67" s="180"/>
-      <c r="F67" s="180"/>
-      <c r="G67" s="180"/>
-      <c r="H67" s="180"/>
-      <c r="I67" s="181"/>
-      <c r="J67" s="179" t="s">
+      <c r="E67" s="181"/>
+      <c r="F67" s="181"/>
+      <c r="G67" s="181"/>
+      <c r="H67" s="181"/>
+      <c r="I67" s="182"/>
+      <c r="J67" s="180" t="s">
         <v>18</v>
       </c>
-      <c r="K67" s="180"/>
-      <c r="L67" s="181"/>
+      <c r="K67" s="181"/>
+      <c r="L67" s="182"/>
       <c r="M67" s="147" t="s">
         <v>19</v>
       </c>
@@ -5459,23 +5462,23 @@
       </c>
     </row>
     <row r="68" spans="2:21" ht="15" customHeight="1">
-      <c r="B68" s="183"/>
-      <c r="C68" s="174"/>
-      <c r="D68" s="176" t="s">
+      <c r="B68" s="190"/>
+      <c r="C68" s="195"/>
+      <c r="D68" s="183" t="s">
         <v>28</v>
       </c>
-      <c r="E68" s="177"/>
-      <c r="F68" s="178"/>
-      <c r="G68" s="176" t="s">
+      <c r="E68" s="184"/>
+      <c r="F68" s="185"/>
+      <c r="G68" s="183" t="s">
         <v>29</v>
       </c>
-      <c r="H68" s="177"/>
-      <c r="I68" s="178"/>
-      <c r="J68" s="176" t="s">
+      <c r="H68" s="184"/>
+      <c r="I68" s="185"/>
+      <c r="J68" s="183" t="s">
         <v>30</v>
       </c>
-      <c r="K68" s="177"/>
-      <c r="L68" s="178"/>
+      <c r="K68" s="184"/>
+      <c r="L68" s="185"/>
       <c r="M68" s="151">
         <v>2</v>
       </c>
@@ -5505,8 +5508,8 @@
       </c>
     </row>
     <row r="69" spans="2:21" ht="31.2">
-      <c r="B69" s="183"/>
-      <c r="C69" s="174"/>
+      <c r="B69" s="190"/>
+      <c r="C69" s="195"/>
       <c r="D69" s="147" t="s">
         <v>31</v>
       </c>
@@ -5551,8 +5554,8 @@
       <c r="U69" s="161"/>
     </row>
     <row r="70" spans="2:21">
-      <c r="B70" s="184"/>
-      <c r="C70" s="175"/>
+      <c r="B70" s="191"/>
+      <c r="C70" s="196"/>
       <c r="D70" s="148">
         <v>0</v>
       </c>
@@ -5597,25 +5600,25 @@
       <c r="U70" s="164"/>
     </row>
     <row r="71" spans="2:21">
-      <c r="B71" s="185" t="s">
+      <c r="B71" s="192" t="s">
         <v>53</v>
       </c>
-      <c r="C71" s="173">
+      <c r="C71" s="197">
         <v>15</v>
       </c>
-      <c r="D71" s="179" t="s">
+      <c r="D71" s="180" t="s">
         <v>17</v>
       </c>
-      <c r="E71" s="180"/>
-      <c r="F71" s="180"/>
-      <c r="G71" s="180"/>
-      <c r="H71" s="180"/>
-      <c r="I71" s="181"/>
-      <c r="J71" s="179" t="s">
+      <c r="E71" s="181"/>
+      <c r="F71" s="181"/>
+      <c r="G71" s="181"/>
+      <c r="H71" s="181"/>
+      <c r="I71" s="182"/>
+      <c r="J71" s="180" t="s">
         <v>18</v>
       </c>
-      <c r="K71" s="180"/>
-      <c r="L71" s="181"/>
+      <c r="K71" s="181"/>
+      <c r="L71" s="182"/>
       <c r="M71" s="147" t="s">
         <v>19</v>
       </c>
@@ -5645,23 +5648,23 @@
       </c>
     </row>
     <row r="72" spans="2:21" ht="15" customHeight="1">
-      <c r="B72" s="183"/>
-      <c r="C72" s="174"/>
-      <c r="D72" s="176" t="s">
+      <c r="B72" s="190"/>
+      <c r="C72" s="195"/>
+      <c r="D72" s="183" t="s">
         <v>28</v>
       </c>
-      <c r="E72" s="177"/>
-      <c r="F72" s="178"/>
-      <c r="G72" s="176" t="s">
+      <c r="E72" s="184"/>
+      <c r="F72" s="185"/>
+      <c r="G72" s="183" t="s">
         <v>29</v>
       </c>
-      <c r="H72" s="177"/>
-      <c r="I72" s="178"/>
-      <c r="J72" s="176" t="s">
+      <c r="H72" s="184"/>
+      <c r="I72" s="185"/>
+      <c r="J72" s="183" t="s">
         <v>30</v>
       </c>
-      <c r="K72" s="177"/>
-      <c r="L72" s="178"/>
+      <c r="K72" s="184"/>
+      <c r="L72" s="185"/>
       <c r="M72" s="151">
         <v>2</v>
       </c>
@@ -5691,8 +5694,8 @@
       </c>
     </row>
     <row r="73" spans="2:21" ht="31.2">
-      <c r="B73" s="183"/>
-      <c r="C73" s="174"/>
+      <c r="B73" s="190"/>
+      <c r="C73" s="195"/>
       <c r="D73" s="147" t="s">
         <v>31</v>
       </c>
@@ -5737,8 +5740,8 @@
       <c r="U73" s="161"/>
     </row>
     <row r="74" spans="2:21">
-      <c r="B74" s="186"/>
-      <c r="C74" s="175"/>
+      <c r="B74" s="193"/>
+      <c r="C74" s="196"/>
       <c r="D74" s="148">
         <v>0</v>
       </c>
@@ -5784,76 +5787,20 @@
     </row>
   </sheetData>
   <mergeCells count="108">
-    <mergeCell ref="D14:L14"/>
-    <mergeCell ref="M14:U14"/>
-    <mergeCell ref="V14:Y14"/>
-    <mergeCell ref="D15:I15"/>
-    <mergeCell ref="J15:L15"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="J16:L16"/>
-    <mergeCell ref="D19:I19"/>
-    <mergeCell ref="J19:L19"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="G20:I20"/>
-    <mergeCell ref="J20:L20"/>
-    <mergeCell ref="D23:I23"/>
-    <mergeCell ref="J23:L23"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="J24:L24"/>
-    <mergeCell ref="D27:I27"/>
-    <mergeCell ref="J27:L27"/>
-    <mergeCell ref="D28:F28"/>
-    <mergeCell ref="G28:I28"/>
-    <mergeCell ref="J28:L28"/>
-    <mergeCell ref="D31:I31"/>
-    <mergeCell ref="J31:L31"/>
-    <mergeCell ref="D32:F32"/>
-    <mergeCell ref="G32:I32"/>
-    <mergeCell ref="J32:L32"/>
-    <mergeCell ref="D35:I35"/>
-    <mergeCell ref="J35:L35"/>
-    <mergeCell ref="D36:F36"/>
-    <mergeCell ref="G36:I36"/>
-    <mergeCell ref="J36:L36"/>
-    <mergeCell ref="D39:I39"/>
-    <mergeCell ref="J39:L39"/>
-    <mergeCell ref="D40:F40"/>
-    <mergeCell ref="G40:I40"/>
-    <mergeCell ref="J40:L40"/>
-    <mergeCell ref="D43:I43"/>
-    <mergeCell ref="J43:L43"/>
-    <mergeCell ref="D44:F44"/>
-    <mergeCell ref="G44:I44"/>
-    <mergeCell ref="J44:L44"/>
-    <mergeCell ref="D47:I47"/>
-    <mergeCell ref="J47:L47"/>
-    <mergeCell ref="D48:F48"/>
-    <mergeCell ref="G48:I48"/>
-    <mergeCell ref="J48:L48"/>
-    <mergeCell ref="D51:I51"/>
-    <mergeCell ref="J51:L51"/>
-    <mergeCell ref="D52:F52"/>
-    <mergeCell ref="G52:I52"/>
-    <mergeCell ref="J52:L52"/>
-    <mergeCell ref="D55:I55"/>
-    <mergeCell ref="J55:L55"/>
-    <mergeCell ref="D56:F56"/>
-    <mergeCell ref="G56:I56"/>
-    <mergeCell ref="J56:L56"/>
-    <mergeCell ref="D59:I59"/>
-    <mergeCell ref="J59:L59"/>
-    <mergeCell ref="D60:F60"/>
-    <mergeCell ref="G60:I60"/>
-    <mergeCell ref="J60:L60"/>
-    <mergeCell ref="D63:I63"/>
-    <mergeCell ref="J63:L63"/>
-    <mergeCell ref="D64:F64"/>
-    <mergeCell ref="G64:I64"/>
-    <mergeCell ref="J64:L64"/>
-    <mergeCell ref="D67:I67"/>
-    <mergeCell ref="J67:L67"/>
+    <mergeCell ref="C55:C58"/>
+    <mergeCell ref="C59:C62"/>
+    <mergeCell ref="C63:C66"/>
+    <mergeCell ref="C67:C70"/>
+    <mergeCell ref="C71:C74"/>
+    <mergeCell ref="C19:C22"/>
+    <mergeCell ref="C23:C26"/>
+    <mergeCell ref="C27:C30"/>
+    <mergeCell ref="C31:C34"/>
+    <mergeCell ref="C35:C38"/>
+    <mergeCell ref="C39:C42"/>
+    <mergeCell ref="C43:C46"/>
+    <mergeCell ref="C47:C50"/>
+    <mergeCell ref="C51:C54"/>
     <mergeCell ref="D68:F68"/>
     <mergeCell ref="G68:I68"/>
     <mergeCell ref="J68:L68"/>
@@ -5878,20 +5825,76 @@
     <mergeCell ref="B67:B70"/>
     <mergeCell ref="B71:B74"/>
     <mergeCell ref="C15:C18"/>
-    <mergeCell ref="C55:C58"/>
-    <mergeCell ref="C59:C62"/>
-    <mergeCell ref="C63:C66"/>
-    <mergeCell ref="C67:C70"/>
-    <mergeCell ref="C71:C74"/>
-    <mergeCell ref="C19:C22"/>
-    <mergeCell ref="C23:C26"/>
-    <mergeCell ref="C27:C30"/>
-    <mergeCell ref="C31:C34"/>
-    <mergeCell ref="C35:C38"/>
-    <mergeCell ref="C39:C42"/>
-    <mergeCell ref="C43:C46"/>
-    <mergeCell ref="C47:C50"/>
-    <mergeCell ref="C51:C54"/>
+    <mergeCell ref="D60:F60"/>
+    <mergeCell ref="G60:I60"/>
+    <mergeCell ref="J60:L60"/>
+    <mergeCell ref="D63:I63"/>
+    <mergeCell ref="J63:L63"/>
+    <mergeCell ref="D64:F64"/>
+    <mergeCell ref="G64:I64"/>
+    <mergeCell ref="J64:L64"/>
+    <mergeCell ref="D67:I67"/>
+    <mergeCell ref="J67:L67"/>
+    <mergeCell ref="D52:F52"/>
+    <mergeCell ref="G52:I52"/>
+    <mergeCell ref="J52:L52"/>
+    <mergeCell ref="D55:I55"/>
+    <mergeCell ref="J55:L55"/>
+    <mergeCell ref="D56:F56"/>
+    <mergeCell ref="G56:I56"/>
+    <mergeCell ref="J56:L56"/>
+    <mergeCell ref="D59:I59"/>
+    <mergeCell ref="J59:L59"/>
+    <mergeCell ref="D44:F44"/>
+    <mergeCell ref="G44:I44"/>
+    <mergeCell ref="J44:L44"/>
+    <mergeCell ref="D47:I47"/>
+    <mergeCell ref="J47:L47"/>
+    <mergeCell ref="D48:F48"/>
+    <mergeCell ref="G48:I48"/>
+    <mergeCell ref="J48:L48"/>
+    <mergeCell ref="D51:I51"/>
+    <mergeCell ref="J51:L51"/>
+    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="G36:I36"/>
+    <mergeCell ref="J36:L36"/>
+    <mergeCell ref="D39:I39"/>
+    <mergeCell ref="J39:L39"/>
+    <mergeCell ref="D40:F40"/>
+    <mergeCell ref="G40:I40"/>
+    <mergeCell ref="J40:L40"/>
+    <mergeCell ref="D43:I43"/>
+    <mergeCell ref="J43:L43"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="G28:I28"/>
+    <mergeCell ref="J28:L28"/>
+    <mergeCell ref="D31:I31"/>
+    <mergeCell ref="J31:L31"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="G32:I32"/>
+    <mergeCell ref="J32:L32"/>
+    <mergeCell ref="D35:I35"/>
+    <mergeCell ref="J35:L35"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="G20:I20"/>
+    <mergeCell ref="J20:L20"/>
+    <mergeCell ref="D23:I23"/>
+    <mergeCell ref="J23:L23"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="J24:L24"/>
+    <mergeCell ref="D27:I27"/>
+    <mergeCell ref="J27:L27"/>
+    <mergeCell ref="D14:L14"/>
+    <mergeCell ref="M14:U14"/>
+    <mergeCell ref="V14:Y14"/>
+    <mergeCell ref="D15:I15"/>
+    <mergeCell ref="J15:L15"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="J16:L16"/>
+    <mergeCell ref="D19:I19"/>
+    <mergeCell ref="J19:L19"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>
@@ -5900,11 +5903,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A2:AG152"/>
+  <dimension ref="A2:AG153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A134" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H96" sqref="H96"/>
+      <selection pane="topRight" activeCell="C144" sqref="C144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
@@ -7609,7 +7612,7 @@
         <v>0</v>
       </c>
       <c r="I96" s="81">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J96" s="81">
         <v>1</v>
@@ -9256,41 +9259,49 @@
     </row>
     <row r="144" spans="2:26">
       <c r="B144" t="s">
+        <v>187</v>
+      </c>
+      <c r="C144" s="1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="145" spans="2:2">
+      <c r="B145" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="146" spans="2:2">
-      <c r="B146" s="135" t="s">
+    <row r="147" spans="2:2">
+      <c r="B147" s="135" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="147" spans="2:2">
-      <c r="B147" t="s">
+    <row r="148" spans="2:2">
+      <c r="B148" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="148" spans="2:2" ht="46.8">
-      <c r="B148" s="1" t="s">
+    <row r="149" spans="2:2" ht="46.8">
+      <c r="B149" s="1" t="s">
         <v>182</v>
-      </c>
-    </row>
-    <row r="149" spans="2:2">
-      <c r="B149" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="150" spans="2:2">
       <c r="B150" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="151" spans="2:2">
       <c r="B151" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="152" spans="2:2">
       <c r="B152" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="153" spans="2:2">
+      <c r="B153" t="s">
         <v>186</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update ExampleCall to print settings
</commit_message>
<xml_diff>
--- a/testbed/OBM/Master_Setup_AC_dense.xlsx
+++ b/testbed/OBM/Master_Setup_AC_dense.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repo\occ-behav-demand-flex\testbed\OBM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4AE69E6-D6A8-4CE0-84FD-0F63A1A95793}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B694727-C398-4F9B-BB5F-3FE2339B4B6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="12456" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5907,7 +5907,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A84" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I103" sqref="I103"/>
+      <selection pane="topRight" activeCell="O103" sqref="O103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
@@ -7609,10 +7609,10 @@
         <v>0</v>
       </c>
       <c r="H96" s="81">
+        <v>0</v>
+      </c>
+      <c r="I96" s="81">
         <v>2</v>
-      </c>
-      <c r="I96" s="81">
-        <v>0</v>
       </c>
       <c r="J96" s="81">
         <v>0</v>
@@ -9262,7 +9262,7 @@
         <v>187</v>
       </c>
       <c r="C144" s="1">
-        <v>120</v>
+        <v>60</v>
       </c>
     </row>
     <row r="145" spans="2:2">

</xml_diff>

<commit_message>
update postprocess and analysis algorithms
</commit_message>
<xml_diff>
--- a/testbed/OBM/Master_Setup_AC_dense.xlsx
+++ b/testbed/OBM/Master_Setup_AC_dense.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repo\occ-behav-demand-flex\testbed\OBM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B694727-C398-4F9B-BB5F-3FE2339B4B6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC646992-5493-42E1-B6D9-D8FFC8320B9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="12456" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5905,9 +5905,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:AG153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="O103" sqref="O103"/>
+      <selection pane="topRight" activeCell="O96" sqref="O96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
@@ -7612,10 +7612,10 @@
         <v>0</v>
       </c>
       <c r="I96" s="81">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J96" s="81">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K96" s="81">
         <v>0</v>

</xml_diff>